<commit_message>
Update with chlorophyll a run from 1-9-24
</commit_message>
<xml_diff>
--- a/data/raw/LowerPoudre_StreamChem_2023.xlsx
+++ b/data/raw/LowerPoudre_StreamChem_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samstruthers/Documents/fork_yeah/PWQN_chemistry_data/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65886AC-D40A-1A4A-BBF9-9A3B26938FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD246D2-808D-F045-9107-80812F12B776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36180" yWindow="-1360" windowWidth="30100" windowHeight="15840" xr2:uid="{03A855A3-FAD4-4527-9341-9B9D95EAB350}"/>
+    <workbookView xWindow="33840" yWindow="500" windowWidth="32300" windowHeight="16940" xr2:uid="{03A855A3-FAD4-4527-9341-9B9D95EAB350}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="170">
   <si>
     <t>IDNo</t>
   </si>
@@ -245,9 +245,6 @@
     <t>DUPLICATE</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>TSS and Turb Confirmed, Storm?</t>
   </si>
   <si>
@@ -483,9 +480,6 @@
   </si>
   <si>
     <t>archery_111623</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>TSS and Turb Confirmed</t>
@@ -1017,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4767B9A8-4210-4712-BEE2-4A2F20C57D9A}">
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C39" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1027,14 +1021,14 @@
     <col min="2" max="2" width="44" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="8" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11" style="8" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="4.83203125" style="8" customWidth="1"/>
     <col min="13" max="15" width="4.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.5" style="8" bestFit="1" customWidth="1"/>
@@ -1053,65 +1047,65 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.15">
       <c r="H1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="L1" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P1" s="21"/>
       <c r="Q1" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="S1" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="R1" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>165</v>
-      </c>
       <c r="T1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="19" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -1137,13 +1131,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>7</v>
@@ -1215,7 +1209,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" s="4">
         <v>45180</v>
@@ -1296,7 +1290,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="4">
         <v>45180</v>
@@ -1377,7 +1371,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" s="4">
         <v>45180</v>
@@ -1458,7 +1452,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E6" s="4">
         <v>45180</v>
@@ -1539,7 +1533,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="4">
         <v>45180</v>
@@ -1782,7 +1776,7 @@
         <v>58</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" s="4">
         <v>45198</v>
@@ -1855,7 +1849,7 @@
         <v>53.158000000000001</v>
       </c>
       <c r="AC10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.15">
@@ -1869,7 +1863,7 @@
         <v>59</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="4">
         <v>45198</v>
@@ -1942,7 +1936,7 @@
         <v>133.822</v>
       </c>
       <c r="AC11" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.15">
@@ -1956,7 +1950,7 @@
         <v>60</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" s="4">
         <v>45198</v>
@@ -2029,7 +2023,7 @@
         <v>205.608</v>
       </c>
       <c r="AC12" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.15">
@@ -2043,7 +2037,7 @@
         <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E13" s="4">
         <v>45198</v>
@@ -2116,7 +2110,7 @@
         <v>478.62</v>
       </c>
       <c r="AC13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.15">
@@ -2130,7 +2124,7 @@
         <v>62</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" s="4">
         <v>45198</v>
@@ -2203,7 +2197,7 @@
         <v>555.77800000000002</v>
       </c>
       <c r="AC14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.15">
@@ -2217,7 +2211,7 @@
         <v>63</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" s="4">
         <v>45202</v>
@@ -2290,7 +2284,7 @@
         <v>54.682000000000002</v>
       </c>
       <c r="AC15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.15">
@@ -2304,7 +2298,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="4">
         <v>45202</v>
@@ -2377,7 +2371,7 @@
         <v>173.39</v>
       </c>
       <c r="AC16" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.15">
@@ -2391,7 +2385,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="4">
         <v>45202</v>
@@ -2464,7 +2458,7 @@
         <v>185.054</v>
       </c>
       <c r="AC17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.15">
@@ -2478,7 +2472,7 @@
         <v>65</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E18" s="4">
         <v>45202</v>
@@ -2563,7 +2557,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E19" s="4">
         <v>45202</v>
@@ -2648,7 +2642,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E20" s="4">
         <v>45202</v>
@@ -2660,12 +2654,8 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="H20" s="7"/>
-      <c r="I20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
       <c r="K20" s="7">
         <v>16.57</v>
       </c>
@@ -2724,13 +2714,13 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>57</v>
@@ -2805,13 +2795,13 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>57</v>
@@ -2892,13 +2882,13 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>57</v>
@@ -2979,16 +2969,16 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E24" s="10">
         <v>45232</v>
@@ -3066,16 +3056,16 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="E25" s="10">
         <v>45232</v>
@@ -3153,16 +3143,16 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="E26" s="10">
         <v>45232</v>
@@ -3240,16 +3230,16 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E27" s="10">
         <v>45232</v>
@@ -3327,16 +3317,16 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E28" s="10">
         <v>45232</v>
@@ -3347,9 +3337,7 @@
       <c r="G28" s="6">
         <v>0.76736111111111116</v>
       </c>
-      <c r="H28" s="20" t="s">
-        <v>149</v>
-      </c>
+      <c r="H28" s="20"/>
       <c r="I28" s="20">
         <v>371.2</v>
       </c>
@@ -3414,13 +3402,13 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>57</v>
@@ -3449,7 +3437,9 @@
       <c r="L29" s="7">
         <v>0.29411764705879112</v>
       </c>
-      <c r="M29" s="7"/>
+      <c r="M29" s="7">
+        <v>0.47</v>
+      </c>
       <c r="N29" s="7">
         <v>3.81</v>
       </c>
@@ -3499,16 +3489,16 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30" s="10">
         <v>45237</v>
@@ -3534,7 +3524,9 @@
       <c r="L30" s="7">
         <v>0.58252427184459599</v>
       </c>
-      <c r="M30" s="7"/>
+      <c r="M30" s="7">
+        <v>1.1299999999999999</v>
+      </c>
       <c r="N30" s="7">
         <v>4.359</v>
       </c>
@@ -3584,16 +3576,16 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="10">
         <v>45237</v>
@@ -3619,7 +3611,9 @@
       <c r="L31" s="7">
         <v>3.5576923076923426</v>
       </c>
-      <c r="M31" s="7"/>
+      <c r="M31" s="7">
+        <v>2.8</v>
+      </c>
       <c r="N31" s="7">
         <v>4.7735000000000003</v>
       </c>
@@ -3669,16 +3663,16 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E32" s="10">
         <v>45237</v>
@@ -3704,7 +3698,9 @@
       <c r="L32" s="7">
         <v>2.4509803921568105</v>
       </c>
-      <c r="M32" s="7"/>
+      <c r="M32" s="7">
+        <v>3.19</v>
+      </c>
       <c r="N32" s="7">
         <v>5.23</v>
       </c>
@@ -3751,21 +3747,21 @@
         <v>974.24400000000003</v>
       </c>
       <c r="AC32" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="10">
         <v>45237</v>
@@ -3791,7 +3787,9 @@
       <c r="L33" s="7">
         <v>6.2068965517241113</v>
       </c>
-      <c r="M33" s="7"/>
+      <c r="M33" s="7">
+        <v>2.5499999999999998</v>
+      </c>
       <c r="N33" s="7">
         <v>4.9424999999999999</v>
       </c>
@@ -3841,16 +3839,16 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="E34" s="10">
         <v>45237</v>
@@ -3876,7 +3874,9 @@
       <c r="L34" s="7">
         <v>1.8446601941747696</v>
       </c>
-      <c r="M34" s="7"/>
+      <c r="M34" s="7">
+        <v>1.5</v>
+      </c>
       <c r="N34" s="7">
         <v>5.9499999999999993</v>
       </c>
@@ -3926,16 +3926,16 @@
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E35" s="10">
         <v>45237</v>
@@ -3961,7 +3961,9 @@
       <c r="L35" s="7">
         <v>7.1844660194175463</v>
       </c>
-      <c r="M35" s="7"/>
+      <c r="M35" s="7">
+        <v>1.82</v>
+      </c>
       <c r="N35" s="7">
         <v>5.5149999999999997</v>
       </c>
@@ -4011,13 +4013,13 @@
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>57</v>
@@ -4046,7 +4048,9 @@
       <c r="L36" s="7">
         <v>0.49504950495044098</v>
       </c>
-      <c r="M36" s="7"/>
+      <c r="M36" s="7">
+        <v>0.38</v>
+      </c>
       <c r="N36" s="7">
         <v>3.7389999999999999</v>
       </c>
@@ -4096,16 +4100,16 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E37" s="10">
         <v>45239</v>
@@ -4131,7 +4135,9 @@
       <c r="L37" s="7">
         <v>0.97087378640766009</v>
       </c>
-      <c r="M37" s="7"/>
+      <c r="M37" s="7">
+        <v>1.51</v>
+      </c>
       <c r="N37" s="7">
         <v>4.5010000000000003</v>
       </c>
@@ -4181,16 +4187,16 @@
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" s="10">
         <v>45239</v>
@@ -4216,7 +4222,9 @@
       <c r="L38" s="7">
         <v>2.7450980392156015</v>
       </c>
-      <c r="M38" s="7"/>
+      <c r="M38" s="7">
+        <v>2.2400000000000002</v>
+      </c>
       <c r="N38" s="7">
         <v>3.9020000000000001</v>
       </c>
@@ -4266,16 +4274,16 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E39" s="10">
         <v>45239</v>
@@ -4301,7 +4309,9 @@
       <c r="L39" s="7">
         <v>2.0909090909090624</v>
       </c>
-      <c r="M39" s="7"/>
+      <c r="M39" s="7">
+        <v>2.95</v>
+      </c>
       <c r="N39" s="7">
         <v>4.3149999999999995</v>
       </c>
@@ -4351,16 +4361,16 @@
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E40" s="10">
         <v>45239</v>
@@ -4386,7 +4396,9 @@
       <c r="L40" s="7">
         <v>26.909090909090974</v>
       </c>
-      <c r="M40" s="7"/>
+      <c r="M40" s="7">
+        <v>1.1399999999999999</v>
+      </c>
       <c r="N40" s="7">
         <v>4.0404999999999998</v>
       </c>
@@ -4436,16 +4448,16 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E41" s="10">
         <v>45239</v>
@@ -4471,7 +4483,9 @@
       <c r="L41" s="7">
         <v>3.9603960396039639</v>
       </c>
-      <c r="M41" s="7"/>
+      <c r="M41" s="7">
+        <v>1.55</v>
+      </c>
       <c r="N41" s="7">
         <v>4.9335000000000004</v>
       </c>
@@ -4521,13 +4535,13 @@
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>57</v>
@@ -4556,7 +4570,9 @@
       <c r="L42" s="7">
         <v>0.79999999999991189</v>
       </c>
-      <c r="M42" s="7"/>
+      <c r="M42" s="7">
+        <v>0.39</v>
+      </c>
       <c r="N42" s="7">
         <v>3.907</v>
       </c>
@@ -4606,16 +4622,16 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E43" s="10">
         <v>45244</v>
@@ -4641,7 +4657,9 @@
       <c r="L43" s="7">
         <v>10.31249999999979</v>
       </c>
-      <c r="M43" s="7"/>
+      <c r="M43" s="7">
+        <v>1.22</v>
+      </c>
       <c r="N43" s="7">
         <v>4.7984999999999998</v>
       </c>
@@ -4688,21 +4706,21 @@
         <v>48.49</v>
       </c>
       <c r="AC43" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E44" s="10">
         <v>45244</v>
@@ -4728,7 +4746,9 @@
       <c r="L44" s="7">
         <v>2.4742268041238966</v>
       </c>
-      <c r="M44" s="7"/>
+      <c r="M44" s="7">
+        <v>2.35</v>
+      </c>
       <c r="N44" s="7">
         <v>6.41</v>
       </c>
@@ -4778,16 +4798,16 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E45" s="10">
         <v>45244</v>
@@ -4813,7 +4833,9 @@
       <c r="L45" s="7">
         <v>4.0999999999999925</v>
       </c>
-      <c r="M45" s="7"/>
+      <c r="M45" s="7">
+        <v>2.78</v>
+      </c>
       <c r="N45" s="7">
         <v>4.8304999999999998</v>
       </c>
@@ -4863,16 +4885,16 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E46" s="10">
         <v>45244</v>
@@ -4898,7 +4920,9 @@
       <c r="L46" s="7">
         <v>54.699999999999903</v>
       </c>
-      <c r="M46" s="7"/>
+      <c r="M46" s="7">
+        <v>3.17</v>
+      </c>
       <c r="N46" s="7">
         <v>4.8230000000000004</v>
       </c>
@@ -4948,16 +4972,16 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E47" s="10">
         <v>45244</v>
@@ -4983,7 +5007,9 @@
       <c r="L47" s="7">
         <v>3.8000000000000256</v>
       </c>
-      <c r="M47" s="7"/>
+      <c r="M47" s="7">
+        <v>1.88</v>
+      </c>
       <c r="N47" s="7">
         <v>5.1349999999999998</v>
       </c>
@@ -5033,16 +5059,16 @@
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E48" s="10">
         <v>45244</v>
@@ -5068,7 +5094,9 @@
       <c r="L48" s="7">
         <v>4.0816326530612281</v>
       </c>
-      <c r="M48" s="7"/>
+      <c r="M48" s="7">
+        <v>2.16</v>
+      </c>
       <c r="N48" s="7">
         <v>5.09</v>
       </c>
@@ -5118,13 +5146,13 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>57</v>
@@ -5153,7 +5181,9 @@
       <c r="L49" s="7">
         <v>0.20202020202017978</v>
       </c>
-      <c r="M49" s="7"/>
+      <c r="M49" s="7">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="N49" s="7">
         <v>2.4510000000000001</v>
       </c>
@@ -5203,16 +5233,16 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" s="10">
         <v>45246</v>
@@ -5238,7 +5268,9 @@
       <c r="L50" s="7">
         <v>0.90909090909080903</v>
       </c>
-      <c r="M50" s="7"/>
+      <c r="M50" s="7">
+        <v>1.3</v>
+      </c>
       <c r="N50" s="7">
         <v>2.87</v>
       </c>
@@ -5288,16 +5320,16 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E51" s="10">
         <v>45246</v>
@@ -5323,7 +5355,9 @@
       <c r="L51" s="7">
         <v>3.3000000000000806</v>
       </c>
-      <c r="M51" s="7"/>
+      <c r="M51" s="7">
+        <v>3.69</v>
+      </c>
       <c r="N51" s="7">
         <v>3.6379999999999999</v>
       </c>
@@ -5373,16 +5407,16 @@
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E52" s="10">
         <v>45246</v>
@@ -5408,7 +5442,9 @@
       <c r="L52" s="7">
         <v>2.0000000000000018</v>
       </c>
-      <c r="M52" s="7"/>
+      <c r="M52" s="7">
+        <v>4.95</v>
+      </c>
       <c r="N52" s="7">
         <v>3.6629999999999998</v>
       </c>
@@ -5455,21 +5491,21 @@
         <v>631.1</v>
       </c>
       <c r="AC52" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E53" s="10">
         <v>45246</v>
@@ -5495,7 +5531,9 @@
       <c r="L53" s="7">
         <v>2.0408163265306141</v>
       </c>
-      <c r="M53" s="7"/>
+      <c r="M53" s="7">
+        <v>3.39</v>
+      </c>
       <c r="N53" s="7">
         <v>4.0030000000000001</v>
       </c>
@@ -5545,16 +5583,16 @@
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E54" s="10">
         <v>45246</v>
@@ -5580,7 +5618,9 @@
       <c r="L54" s="7">
         <v>1.6000000000000458</v>
       </c>
-      <c r="M54" s="7"/>
+      <c r="M54" s="7">
+        <v>2.2599999999999998</v>
+      </c>
       <c r="N54" s="7">
         <v>3.8050000000000002</v>
       </c>
@@ -5630,16 +5670,16 @@
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E55" s="10">
         <v>45246</v>
@@ -5665,7 +5705,9 @@
       <c r="L55" s="7">
         <v>1.5000000000000568</v>
       </c>
-      <c r="M55" s="7"/>
+      <c r="M55" s="7">
+        <v>2.38</v>
+      </c>
       <c r="N55" s="7">
         <v>4.1719999999999997</v>
       </c>
@@ -5715,16 +5757,16 @@
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E56" s="12">
         <v>45265</v>
@@ -5746,7 +5788,9 @@
       </c>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
+      <c r="M56" s="7">
+        <v>1.55</v>
+      </c>
       <c r="N56" s="7">
         <v>2.94</v>
       </c>
@@ -5796,16 +5840,16 @@
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E57" s="12">
         <v>45265</v>
@@ -5827,7 +5871,9 @@
       </c>
       <c r="K57" s="7"/>
       <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
+      <c r="M57" s="7">
+        <v>1.5</v>
+      </c>
       <c r="N57" s="7">
         <v>3.1619999999999999</v>
       </c>
@@ -5877,16 +5923,16 @@
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E58" s="12">
         <v>45265</v>
@@ -5908,7 +5954,9 @@
       </c>
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
+      <c r="M58" s="7">
+        <v>1.94</v>
+      </c>
       <c r="N58" s="7">
         <v>3.1669999999999998</v>
       </c>
@@ -5958,16 +6006,16 @@
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E59" s="12">
         <v>45265</v>
@@ -5989,7 +6037,9 @@
       </c>
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
+      <c r="M59" s="7">
+        <v>1.54</v>
+      </c>
       <c r="N59" s="7">
         <v>3.8170000000000002</v>
       </c>
@@ -6039,16 +6089,16 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E60" s="12">
         <v>45265</v>
@@ -6070,7 +6120,9 @@
       </c>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
+      <c r="M60" s="7">
+        <v>1.61</v>
+      </c>
       <c r="N60" s="7">
         <v>3.9209999999999998</v>
       </c>

</xml_diff>